<commit_message>
Update 16S tree with Sanger contig sequence
</commit_message>
<xml_diff>
--- a/isolation/DTD_run2.xlsx
+++ b/isolation/DTD_run2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rprops\Documents\Limno_CoolingWater\isolation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rprops\Documents\Ramlibacter--CW\isolation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="37">
   <si>
     <t>A01</t>
   </si>
@@ -125,13 +125,16 @@
     <t>To analyse</t>
   </si>
   <si>
-    <t>Sanger sequence</t>
-  </si>
-  <si>
     <t>Classification</t>
   </si>
   <si>
     <t>Extracted (succesfully)</t>
+  </si>
+  <si>
+    <t>Contig_2: Ramlibacter</t>
+  </si>
+  <si>
+    <t>Sanger_ID</t>
   </si>
 </sst>
 </file>
@@ -469,7 +472,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="C18" sqref="C18:H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,7 +481,7 @@
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -489,13 +492,13 @@
         <v>31</v>
       </c>
       <c r="G1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" t="s">
         <v>33</v>
-      </c>
-      <c r="I1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -719,6 +722,9 @@
       <c r="G14" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="H14" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -750,7 +756,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -765,7 +771,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
@@ -788,8 +794,14 @@
       <c r="G18" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" s="2">
+        <v>2</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -804,7 +816,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -819,7 +831,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
@@ -837,7 +849,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
@@ -855,7 +867,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
@@ -878,8 +890,11 @@
       <c r="G23" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
@@ -902,8 +917,11 @@
       <c r="G24" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>23</v>
       </c>
@@ -925,6 +943,9 @@
       </c>
       <c r="G25" s="2" t="s">
         <v>30</v>
+      </c>
+      <c r="H25" s="2">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started module completeness analysis for Ramlibacter MAG
</commit_message>
<xml_diff>
--- a/isolation/DTD_run2.xlsx
+++ b/isolation/DTD_run2.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="42">
   <si>
     <t>A01</t>
   </si>
@@ -135,13 +135,28 @@
   </si>
   <si>
     <t>Sanger_ID</t>
+  </si>
+  <si>
+    <t>Contig_5: Reyranella</t>
+  </si>
+  <si>
+    <t>Contig_4: Reyranella</t>
+  </si>
+  <si>
+    <t>Contig_1: Acidibacter ferrireducens</t>
+  </si>
+  <si>
+    <t>Contig_3: Phenylobacterium</t>
+  </si>
+  <si>
+    <t>In cultivation - 7/12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,8 +171,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -167,6 +189,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -179,17 +207,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="11" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="11" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -469,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18:H18"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,10 +513,11 @@
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E1" t="s">
         <v>32</v>
       </c>
@@ -500,8 +533,11 @@
       <c r="I1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -516,7 +552,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -531,7 +567,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -546,7 +582,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -564,7 +600,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -582,7 +618,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -600,7 +636,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -615,7 +651,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -630,7 +666,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -645,7 +681,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -663,7 +699,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -681,7 +717,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -699,7 +735,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -725,8 +761,14 @@
       <c r="H14" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -740,8 +782,11 @@
       <c r="D15" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -755,8 +800,11 @@
       <c r="D16" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -770,38 +818,44 @@
       <c r="D17" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="J17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="4">
         <v>530</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="5">
         <f t="shared" si="0"/>
         <v>1060000</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E18" t="s">
-        <v>29</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H18" s="2">
+      <c r="E18" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H18" s="4">
         <v>2</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="I18" s="4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -815,8 +869,11 @@
       <c r="D19" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -831,7 +888,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
@@ -849,7 +906,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
@@ -867,7 +924,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
@@ -893,8 +950,14 @@
       <c r="H23" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I23" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
@@ -920,8 +983,14 @@
       <c r="H24" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I24" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>23</v>
       </c>
@@ -946,6 +1015,12 @@
       </c>
       <c r="H25" s="2">
         <v>5</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>